<commit_message>
It is now uploading the data from the excel file to the DB
Now it is parsing the Data from the file and making an object to upload to the DB. Right now it is not allowing any sort of updating, so if you make changes to the Excel sheet, you need to delete the DB and run the program again.

I added the Corporate controller and view so I can display what is inside the DB.

Final steps for the Database on this project is to allow updating.
</commit_message>
<xml_diff>
--- a/ExcelSheets/Tax_List_Sample.xlsx
+++ b/ExcelSheets/Tax_List_Sample.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gclafli1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cutte\Desktop\School\Fall2018\WebAppDevelopment\TaxWebApp\TaxWebApp\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE501960-EB13-47A8-BE80-805DB35E9879}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22896" windowHeight="14196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personals " sheetId="1" r:id="rId1"/>
     <sheet name="Corporate" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="155">
   <si>
     <t>NUMBER</t>
   </si>
@@ -495,7 +501,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,7 +631,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -903,29 +909,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J237"/>
   <sheetViews>
-    <sheetView topLeftCell="D51" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="10.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -955,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3">
         <v>18001</v>
@@ -963,7 +969,9 @@
       <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="6">
         <v>43101</v>
@@ -981,7 +989,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3">
         <f>1+B2</f>
@@ -1008,7 +1016,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B67" si="0">1+B3</f>
@@ -1035,7 +1043,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
@@ -1066,7 +1074,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
@@ -1093,7 +1101,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
@@ -1120,7 +1128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
@@ -1149,7 +1157,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
@@ -1176,7 +1184,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
@@ -1205,7 +1213,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
@@ -1236,7 +1244,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
@@ -1263,7 +1271,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
@@ -1290,7 +1298,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <f t="shared" si="0"/>
@@ -1316,7 +1324,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <f t="shared" si="0"/>
@@ -1343,7 +1351,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <f t="shared" si="0"/>
@@ -1370,7 +1378,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
@@ -1397,7 +1405,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
@@ -1428,7 +1436,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
@@ -1455,7 +1463,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -1482,7 +1490,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -1509,7 +1517,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3">
         <f t="shared" si="0"/>
@@ -1536,7 +1544,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <f t="shared" si="0"/>
@@ -1562,7 +1570,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3">
         <f t="shared" si="0"/>
@@ -1589,7 +1597,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3">
         <f t="shared" si="0"/>
@@ -1618,7 +1626,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3">
         <f t="shared" si="0"/>
@@ -1647,7 +1655,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3">
         <f t="shared" si="0"/>
@@ -1676,7 +1684,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3">
         <f t="shared" si="0"/>
@@ -1703,7 +1711,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3">
         <f t="shared" si="0"/>
@@ -1730,7 +1738,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3">
         <f t="shared" si="0"/>
@@ -1757,7 +1765,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3">
         <f t="shared" si="0"/>
@@ -1784,7 +1792,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3">
         <f t="shared" si="0"/>
@@ -1811,7 +1819,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3">
         <f t="shared" si="0"/>
@@ -1838,7 +1846,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3">
         <f t="shared" si="0"/>
@@ -1865,7 +1873,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3">
         <f t="shared" si="0"/>
@@ -1894,7 +1902,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3">
         <f t="shared" si="0"/>
@@ -1921,7 +1929,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3">
         <f t="shared" si="0"/>
@@ -1948,7 +1956,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3">
         <f t="shared" si="0"/>
@@ -1975,7 +1983,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3">
         <f t="shared" si="0"/>
@@ -2002,7 +2010,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3">
         <f t="shared" si="0"/>
@@ -2029,7 +2037,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3">
         <f t="shared" si="0"/>
@@ -2056,7 +2064,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3">
         <f t="shared" si="0"/>
@@ -2083,7 +2091,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3">
         <f t="shared" si="0"/>
@@ -2110,7 +2118,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3">
         <f t="shared" si="0"/>
@@ -2137,7 +2145,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3">
         <f t="shared" si="0"/>
@@ -2164,7 +2172,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3">
         <f t="shared" si="0"/>
@@ -2191,7 +2199,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3">
         <f t="shared" si="0"/>
@@ -2220,7 +2228,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3">
         <f t="shared" si="0"/>
@@ -2245,7 +2253,7 @@
       </c>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3">
         <f t="shared" si="0"/>
@@ -2272,7 +2280,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3">
         <f t="shared" si="0"/>
@@ -2301,7 +2309,7 @@
       </c>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3">
         <f t="shared" si="0"/>
@@ -2326,7 +2334,7 @@
       </c>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3">
         <f t="shared" si="0"/>
@@ -2353,7 +2361,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
@@ -2379,7 +2387,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
@@ -2404,7 +2412,7 @@
       </c>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
@@ -2429,7 +2437,7 @@
       </c>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
@@ -2454,7 +2462,7 @@
       </c>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
@@ -2481,7 +2489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
@@ -2508,7 +2516,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
@@ -2533,7 +2541,7 @@
       </c>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
@@ -2558,7 +2566,7 @@
       </c>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
@@ -2583,7 +2591,7 @@
       </c>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
@@ -2612,7 +2620,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
@@ -2639,7 +2647,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
@@ -2666,7 +2674,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
@@ -2695,7 +2703,7 @@
       </c>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
@@ -2720,7 +2728,7 @@
       </c>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
@@ -2743,7 +2751,7 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3">
         <f t="shared" ref="B68:B131" si="1">1+B67</f>
@@ -2770,7 +2778,7 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3">
         <f t="shared" si="1"/>
@@ -2793,7 +2801,7 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3">
         <f t="shared" si="1"/>
@@ -2816,7 +2824,7 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3">
         <f t="shared" si="1"/>
@@ -2841,7 +2849,7 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3">
         <f t="shared" si="1"/>
@@ -2864,7 +2872,7 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3">
         <f t="shared" si="1"/>
@@ -2887,7 +2895,7 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3">
         <f t="shared" si="1"/>
@@ -2910,7 +2918,7 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3">
         <f t="shared" si="1"/>
@@ -2933,7 +2941,7 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3">
         <f t="shared" si="1"/>
@@ -2956,7 +2964,7 @@
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3">
         <f t="shared" si="1"/>
@@ -2979,7 +2987,7 @@
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3">
         <f t="shared" si="1"/>
@@ -3002,7 +3010,7 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3">
         <f t="shared" si="1"/>
@@ -3025,7 +3033,7 @@
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3">
         <f t="shared" si="1"/>
@@ -3050,7 +3058,7 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3">
         <f t="shared" si="1"/>
@@ -3073,7 +3081,7 @@
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3">
         <f t="shared" si="1"/>
@@ -3096,7 +3104,7 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3">
         <f t="shared" si="1"/>
@@ -3119,7 +3127,7 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3">
         <f t="shared" si="1"/>
@@ -3142,7 +3150,7 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3">
         <f t="shared" si="1"/>
@@ -3165,7 +3173,7 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3">
         <f t="shared" si="1"/>
@@ -3186,7 +3194,7 @@
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3">
         <f t="shared" si="1"/>
@@ -3206,7 +3214,7 @@
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3">
         <f t="shared" si="1"/>
@@ -3226,7 +3234,7 @@
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3">
         <f t="shared" si="1"/>
@@ -3247,7 +3255,7 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3">
         <f t="shared" si="1"/>
@@ -3268,7 +3276,7 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3">
         <f t="shared" si="1"/>
@@ -3291,7 +3299,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3">
         <f t="shared" si="1"/>
@@ -3312,7 +3320,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3">
         <f t="shared" si="1"/>
@@ -3333,7 +3341,7 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3">
         <f t="shared" si="1"/>
@@ -3354,7 +3362,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3">
         <f t="shared" si="1"/>
@@ -3379,7 +3387,7 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3">
         <f t="shared" si="1"/>
@@ -3400,7 +3408,7 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3">
         <f t="shared" si="1"/>
@@ -3421,7 +3429,7 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3">
         <f t="shared" si="1"/>
@@ -3442,7 +3450,7 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3">
         <f t="shared" si="1"/>
@@ -3463,7 +3471,7 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3">
         <f t="shared" si="1"/>
@@ -3486,7 +3494,7 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3">
         <f t="shared" si="1"/>
@@ -3507,7 +3515,7 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3">
         <f t="shared" si="1"/>
@@ -3522,7 +3530,7 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3">
         <f t="shared" si="1"/>
@@ -3537,7 +3545,7 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3">
         <f t="shared" si="1"/>
@@ -3552,7 +3560,7 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3">
         <f t="shared" si="1"/>
@@ -3567,7 +3575,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3">
         <f t="shared" si="1"/>
@@ -3582,7 +3590,7 @@
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3">
         <f t="shared" si="1"/>
@@ -3597,7 +3605,7 @@
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3">
         <f t="shared" si="1"/>
@@ -3612,7 +3620,7 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3">
         <f t="shared" si="1"/>
@@ -3627,7 +3635,7 @@
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3">
         <f t="shared" si="1"/>
@@ -3642,7 +3650,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3">
         <f t="shared" si="1"/>
@@ -3657,7 +3665,7 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3">
         <f t="shared" si="1"/>
@@ -3672,7 +3680,7 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3">
         <f t="shared" si="1"/>
@@ -3687,7 +3695,7 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3">
         <f t="shared" si="1"/>
@@ -3702,7 +3710,7 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3">
         <f t="shared" si="1"/>
@@ -3717,7 +3725,7 @@
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3">
         <f t="shared" si="1"/>
@@ -3732,7 +3740,7 @@
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3">
         <f t="shared" si="1"/>
@@ -3747,7 +3755,7 @@
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3">
         <f t="shared" si="1"/>
@@ -3762,7 +3770,7 @@
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3">
         <f t="shared" si="1"/>
@@ -3777,7 +3785,7 @@
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3">
         <f t="shared" si="1"/>
@@ -3792,7 +3800,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3">
         <f t="shared" si="1"/>
@@ -3807,7 +3815,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3">
         <f t="shared" si="1"/>
@@ -3822,7 +3830,7 @@
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3">
         <f t="shared" si="1"/>
@@ -3837,7 +3845,7 @@
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3">
         <f t="shared" si="1"/>
@@ -3852,7 +3860,7 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3">
         <f t="shared" si="1"/>
@@ -3867,7 +3875,7 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3">
         <f t="shared" si="1"/>
@@ -3882,7 +3890,7 @@
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3">
         <f t="shared" si="1"/>
@@ -3897,7 +3905,7 @@
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3">
         <f t="shared" si="1"/>
@@ -3912,7 +3920,7 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3">
         <f t="shared" si="1"/>
@@ -3927,7 +3935,7 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3">
         <f t="shared" si="1"/>
@@ -3942,7 +3950,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3">
         <f t="shared" si="1"/>
@@ -3957,7 +3965,7 @@
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3">
         <f t="shared" ref="B132:B195" si="2">1+B131</f>
@@ -3972,7 +3980,7 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3">
         <f t="shared" si="2"/>
@@ -3987,7 +3995,7 @@
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3">
         <f t="shared" si="2"/>
@@ -4002,7 +4010,7 @@
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3">
         <f t="shared" si="2"/>
@@ -4017,7 +4025,7 @@
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3">
         <f t="shared" si="2"/>
@@ -4032,7 +4040,7 @@
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3">
         <f t="shared" si="2"/>
@@ -4047,7 +4055,7 @@
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3">
         <f t="shared" si="2"/>
@@ -4062,7 +4070,7 @@
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3">
         <f t="shared" si="2"/>
@@ -4077,7 +4085,7 @@
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3">
         <f t="shared" si="2"/>
@@ -4092,7 +4100,7 @@
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3">
         <f t="shared" si="2"/>
@@ -4107,7 +4115,7 @@
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3">
         <f t="shared" si="2"/>
@@ -4122,7 +4130,7 @@
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3">
         <f t="shared" si="2"/>
@@ -4137,7 +4145,7 @@
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3">
         <f t="shared" si="2"/>
@@ -4152,7 +4160,7 @@
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3">
         <f t="shared" si="2"/>
@@ -4167,7 +4175,7 @@
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3">
         <f t="shared" si="2"/>
@@ -4182,7 +4190,7 @@
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3">
         <f t="shared" si="2"/>
@@ -4197,7 +4205,7 @@
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3">
         <f t="shared" si="2"/>
@@ -4212,7 +4220,7 @@
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3">
         <f t="shared" si="2"/>
@@ -4227,7 +4235,7 @@
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3">
         <f t="shared" si="2"/>
@@ -4242,7 +4250,7 @@
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3">
         <f t="shared" si="2"/>
@@ -4257,7 +4265,7 @@
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3">
         <f t="shared" si="2"/>
@@ -4272,7 +4280,7 @@
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3">
         <f t="shared" si="2"/>
@@ -4287,7 +4295,7 @@
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3">
         <f t="shared" si="2"/>
@@ -4302,7 +4310,7 @@
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3">
         <f t="shared" si="2"/>
@@ -4317,7 +4325,7 @@
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3">
         <f t="shared" si="2"/>
@@ -4332,7 +4340,7 @@
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="3">
         <f t="shared" si="2"/>
@@ -4347,7 +4355,7 @@
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3">
         <f t="shared" si="2"/>
@@ -4362,7 +4370,7 @@
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3">
         <f t="shared" si="2"/>
@@ -4377,7 +4385,7 @@
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="3">
         <f t="shared" si="2"/>
@@ -4392,7 +4400,7 @@
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="3">
         <f t="shared" si="2"/>
@@ -4407,7 +4415,7 @@
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="3">
         <f t="shared" si="2"/>
@@ -4422,7 +4430,7 @@
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3">
         <f t="shared" si="2"/>
@@ -4437,7 +4445,7 @@
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3">
         <f t="shared" si="2"/>
@@ -4452,7 +4460,7 @@
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3">
         <f t="shared" si="2"/>
@@ -4467,7 +4475,7 @@
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3">
         <f t="shared" si="2"/>
@@ -4482,7 +4490,7 @@
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3">
         <f t="shared" si="2"/>
@@ -4497,7 +4505,7 @@
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3">
         <f t="shared" si="2"/>
@@ -4512,7 +4520,7 @@
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="3">
         <f t="shared" si="2"/>
@@ -4527,7 +4535,7 @@
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="3">
         <f t="shared" si="2"/>
@@ -4542,7 +4550,7 @@
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="3">
         <f t="shared" si="2"/>
@@ -4557,7 +4565,7 @@
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="3">
         <f t="shared" si="2"/>
@@ -4572,7 +4580,7 @@
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="3">
         <f t="shared" si="2"/>
@@ -4587,7 +4595,7 @@
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="3">
         <f t="shared" si="2"/>
@@ -4602,7 +4610,7 @@
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="3">
         <f t="shared" si="2"/>
@@ -4617,7 +4625,7 @@
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="3">
         <f t="shared" si="2"/>
@@ -4632,7 +4640,7 @@
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3">
         <f t="shared" si="2"/>
@@ -4647,7 +4655,7 @@
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3">
         <f t="shared" si="2"/>
@@ -4662,7 +4670,7 @@
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3">
         <f t="shared" si="2"/>
@@ -4677,7 +4685,7 @@
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3">
         <f t="shared" si="2"/>
@@ -4692,7 +4700,7 @@
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="3">
         <f t="shared" si="2"/>
@@ -4707,7 +4715,7 @@
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="3">
         <f t="shared" si="2"/>
@@ -4722,7 +4730,7 @@
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="3">
         <f t="shared" si="2"/>
@@ -4737,7 +4745,7 @@
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="3">
         <f t="shared" si="2"/>
@@ -4752,7 +4760,7 @@
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="3">
         <f t="shared" si="2"/>
@@ -4767,7 +4775,7 @@
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="3">
         <f t="shared" si="2"/>
@@ -4782,7 +4790,7 @@
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="3">
         <f t="shared" si="2"/>
@@ -4797,7 +4805,7 @@
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="3">
         <f t="shared" si="2"/>
@@ -4812,7 +4820,7 @@
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="3">
         <f t="shared" si="2"/>
@@ -4827,7 +4835,7 @@
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="3">
         <f t="shared" si="2"/>
@@ -4842,7 +4850,7 @@
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="3">
         <f t="shared" si="2"/>
@@ -4857,7 +4865,7 @@
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="3">
         <f t="shared" si="2"/>
@@ -4872,7 +4880,7 @@
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="3">
         <f t="shared" si="2"/>
@@ -4887,7 +4895,7 @@
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="3">
         <f t="shared" si="2"/>
@@ -4902,7 +4910,7 @@
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="3">
         <f t="shared" si="2"/>
@@ -4917,7 +4925,7 @@
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="3">
         <f t="shared" ref="B196:B237" si="3">1+B195</f>
@@ -4932,7 +4940,7 @@
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="3">
         <f t="shared" si="3"/>
@@ -4947,7 +4955,7 @@
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="3">
         <f t="shared" si="3"/>
@@ -4962,7 +4970,7 @@
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="3">
         <f t="shared" si="3"/>
@@ -4977,7 +4985,7 @@
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
       <c r="B200" s="3">
         <f t="shared" si="3"/>
@@ -4992,7 +5000,7 @@
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
       <c r="B201" s="3">
         <f t="shared" si="3"/>
@@ -5007,7 +5015,7 @@
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
       <c r="B202" s="3">
         <f t="shared" si="3"/>
@@ -5022,7 +5030,7 @@
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
       <c r="B203" s="3">
         <f t="shared" si="3"/>
@@ -5037,7 +5045,7 @@
       <c r="I203" s="3"/>
       <c r="J203" s="3"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="3">
         <f t="shared" si="3"/>
@@ -5052,7 +5060,7 @@
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
       <c r="B205" s="3">
         <f t="shared" si="3"/>
@@ -5067,7 +5075,7 @@
       <c r="I205" s="3"/>
       <c r="J205" s="3"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
       <c r="B206" s="3">
         <f t="shared" si="3"/>
@@ -5082,7 +5090,7 @@
       <c r="I206" s="3"/>
       <c r="J206" s="3"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
       <c r="B207" s="3">
         <f t="shared" si="3"/>
@@ -5097,7 +5105,7 @@
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
       <c r="B208" s="3">
         <f t="shared" si="3"/>
@@ -5112,7 +5120,7 @@
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
       <c r="B209" s="3">
         <f t="shared" si="3"/>
@@ -5127,7 +5135,7 @@
       <c r="I209" s="3"/>
       <c r="J209" s="3"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
       <c r="B210" s="3">
         <f t="shared" si="3"/>
@@ -5142,7 +5150,7 @@
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
       <c r="B211" s="3">
         <f t="shared" si="3"/>
@@ -5157,7 +5165,7 @@
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
       <c r="B212" s="3">
         <f t="shared" si="3"/>
@@ -5172,7 +5180,7 @@
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
       <c r="B213" s="3">
         <f t="shared" si="3"/>
@@ -5187,7 +5195,7 @@
       <c r="I213" s="3"/>
       <c r="J213" s="3"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2">
         <f t="shared" si="3"/>
@@ -5202,7 +5210,7 @@
       <c r="I214" s="2"/>
       <c r="J214" s="2"/>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2">
         <f t="shared" si="3"/>
@@ -5217,7 +5225,7 @@
       <c r="I215" s="2"/>
       <c r="J215" s="2"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2">
         <f t="shared" si="3"/>
@@ -5232,7 +5240,7 @@
       <c r="I216" s="2"/>
       <c r="J216" s="2"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2">
         <f t="shared" si="3"/>
@@ -5247,7 +5255,7 @@
       <c r="I217" s="2"/>
       <c r="J217" s="2"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2">
         <f t="shared" si="3"/>
@@ -5262,7 +5270,7 @@
       <c r="I218" s="2"/>
       <c r="J218" s="2"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2">
         <f t="shared" si="3"/>
@@ -5277,7 +5285,7 @@
       <c r="I219" s="2"/>
       <c r="J219" s="2"/>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2">
         <f t="shared" si="3"/>
@@ -5292,7 +5300,7 @@
       <c r="I220" s="2"/>
       <c r="J220" s="2"/>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2">
         <f t="shared" si="3"/>
@@ -5307,7 +5315,7 @@
       <c r="I221" s="2"/>
       <c r="J221" s="2"/>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2">
         <f t="shared" si="3"/>
@@ -5322,7 +5330,7 @@
       <c r="I222" s="2"/>
       <c r="J222" s="2"/>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2">
         <f t="shared" si="3"/>
@@ -5337,7 +5345,7 @@
       <c r="I223" s="2"/>
       <c r="J223" s="2"/>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2">
         <f t="shared" si="3"/>
@@ -5352,7 +5360,7 @@
       <c r="I224" s="2"/>
       <c r="J224" s="2"/>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2">
         <f t="shared" si="3"/>
@@ -5367,7 +5375,7 @@
       <c r="I225" s="2"/>
       <c r="J225" s="2"/>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2">
         <f t="shared" si="3"/>
@@ -5382,7 +5390,7 @@
       <c r="I226" s="2"/>
       <c r="J226" s="2"/>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2">
         <f t="shared" si="3"/>
@@ -5397,7 +5405,7 @@
       <c r="I227" s="2"/>
       <c r="J227" s="2"/>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2">
         <f t="shared" si="3"/>
@@ -5412,7 +5420,7 @@
       <c r="I228" s="2"/>
       <c r="J228" s="2"/>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2">
         <f t="shared" si="3"/>
@@ -5427,7 +5435,7 @@
       <c r="I229" s="2"/>
       <c r="J229" s="2"/>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2">
         <f t="shared" si="3"/>
@@ -5442,7 +5450,7 @@
       <c r="I230" s="2"/>
       <c r="J230" s="2"/>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2">
         <f t="shared" si="3"/>
@@ -5457,7 +5465,7 @@
       <c r="I231" s="2"/>
       <c r="J231" s="2"/>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2">
         <f t="shared" si="3"/>
@@ -5472,7 +5480,7 @@
       <c r="I232" s="2"/>
       <c r="J232" s="2"/>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2">
         <f t="shared" si="3"/>
@@ -5487,7 +5495,7 @@
       <c r="I233" s="2"/>
       <c r="J233" s="2"/>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="2">
         <f t="shared" si="3"/>
@@ -5502,7 +5510,7 @@
       <c r="I234" s="2"/>
       <c r="J234" s="2"/>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="2">
         <f t="shared" si="3"/>
@@ -5517,7 +5525,7 @@
       <c r="I235" s="2"/>
       <c r="J235" s="2"/>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="2">
         <f t="shared" si="3"/>
@@ -5532,7 +5540,7 @@
       <c r="I236" s="2"/>
       <c r="J236" s="2"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="2">
         <f t="shared" si="3"/>
@@ -5554,26 +5562,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -5602,7 +5610,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>148</v>
       </c>
@@ -5629,7 +5637,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>149</v>
       </c>
@@ -5657,7 +5665,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>150</v>
       </c>
@@ -5687,7 +5695,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>151</v>
       </c>
@@ -5715,7 +5723,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>149</v>
       </c>
@@ -5743,7 +5751,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>150</v>
       </c>
@@ -5773,7 +5781,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>148</v>
       </c>
@@ -5801,7 +5809,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>149</v>
       </c>
@@ -5829,7 +5837,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>150</v>
       </c>
@@ -5855,7 +5863,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>148</v>
       </c>
@@ -5881,7 +5889,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>151</v>
       </c>
@@ -5909,7 +5917,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>148</v>
       </c>
@@ -5937,7 +5945,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>148</v>
       </c>
@@ -5961,7 +5969,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>149</v>
       </c>
@@ -5989,7 +5997,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>150</v>
       </c>
@@ -6013,7 +6021,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>150</v>
       </c>
@@ -6037,7 +6045,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>148</v>
       </c>
@@ -6061,7 +6069,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>148</v>
       </c>
@@ -6087,7 +6095,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>151</v>
       </c>
@@ -6111,7 +6119,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>150</v>
       </c>
@@ -6135,7 +6143,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
@@ -6151,7 +6159,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -6167,7 +6175,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
@@ -6183,7 +6191,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
@@ -6199,7 +6207,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
@@ -6215,7 +6223,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
@@ -6231,7 +6239,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
@@ -6247,7 +6255,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
@@ -6263,7 +6271,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2">
         <f t="shared" si="0"/>
@@ -6279,7 +6287,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2">
         <f t="shared" si="0"/>
@@ -6295,7 +6303,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2">
         <f t="shared" si="0"/>
@@ -6311,7 +6319,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2">
         <f t="shared" si="0"/>
@@ -6327,7 +6335,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2">
         <f t="shared" si="0"/>
@@ -6343,7 +6351,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2">
         <f t="shared" si="0"/>
@@ -6359,7 +6367,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2">
         <f t="shared" si="0"/>
@@ -6375,7 +6383,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2">
         <f t="shared" si="0"/>
@@ -6391,7 +6399,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2">
         <f t="shared" si="0"/>
@@ -6407,7 +6415,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2">
         <f t="shared" si="0"/>
@@ -6423,7 +6431,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2">
         <f t="shared" si="0"/>
@@ -6439,7 +6447,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2">
         <f t="shared" si="0"/>
@@ -6455,7 +6463,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2">
         <f t="shared" si="0"/>
@@ -6471,7 +6479,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2">
         <f t="shared" si="0"/>
@@ -6487,7 +6495,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2">
         <f t="shared" si="0"/>
@@ -6503,7 +6511,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2">
         <f t="shared" si="0"/>
@@ -6519,7 +6527,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
         <f t="shared" si="0"/>
@@ -6535,7 +6543,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2">
         <f t="shared" si="0"/>
@@ -6551,7 +6559,7 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2">
         <f t="shared" si="0"/>
@@ -6567,7 +6575,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2">
         <f t="shared" si="0"/>
@@ -6583,7 +6591,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2">
         <f t="shared" si="0"/>
@@ -6599,7 +6607,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2">
         <f>1+B50</f>
@@ -6615,7 +6623,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -6628,7 +6636,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -6641,7 +6649,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -6654,7 +6662,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -6667,7 +6675,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -6680,7 +6688,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -6693,7 +6701,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -6706,7 +6714,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -6719,7 +6727,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -6732,7 +6740,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -6745,7 +6753,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -6758,7 +6766,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -6771,7 +6779,7 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -6784,7 +6792,7 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -6797,7 +6805,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -6810,7 +6818,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -6823,7 +6831,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -6836,7 +6844,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -6849,7 +6857,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -6862,7 +6870,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -6875,7 +6883,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -6888,7 +6896,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -6901,7 +6909,7 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -6914,7 +6922,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -6927,7 +6935,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -6940,7 +6948,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -6953,7 +6961,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -6966,7 +6974,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -6979,7 +6987,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -6992,7 +7000,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -7005,7 +7013,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -7018,7 +7026,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -7031,7 +7039,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -7044,7 +7052,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -7057,7 +7065,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -7070,7 +7078,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -7083,7 +7091,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -7096,7 +7104,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -7109,7 +7117,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -7122,7 +7130,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -7135,7 +7143,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -7148,7 +7156,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -7161,7 +7169,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -7174,7 +7182,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -7187,7 +7195,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -7200,7 +7208,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -7213,7 +7221,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -7226,7 +7234,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -7239,7 +7247,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -7252,7 +7260,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -7265,7 +7273,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -7278,7 +7286,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -7291,7 +7299,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7304,7 +7312,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7317,7 +7325,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -7330,7 +7338,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -7343,7 +7351,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -7356,7 +7364,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -7369,7 +7377,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -7382,7 +7390,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -7395,7 +7403,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -7408,7 +7416,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -7421,7 +7429,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -7434,7 +7442,7 @@
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -7447,7 +7455,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -7460,7 +7468,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -7473,7 +7481,7 @@
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -7486,7 +7494,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -7499,7 +7507,7 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -7512,7 +7520,7 @@
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -7525,7 +7533,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -7538,7 +7546,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -7551,7 +7559,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -7564,7 +7572,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -7577,7 +7585,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -7590,7 +7598,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -7603,7 +7611,7 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -7616,7 +7624,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -7629,7 +7637,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -7642,7 +7650,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -7655,7 +7663,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -7668,7 +7676,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -7681,7 +7689,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -7694,7 +7702,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -7707,7 +7715,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -7720,7 +7728,7 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -7733,7 +7741,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -7746,7 +7754,7 @@
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -7759,7 +7767,7 @@
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -7772,7 +7780,7 @@
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -7785,7 +7793,7 @@
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -7798,7 +7806,7 @@
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -7811,7 +7819,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -7824,7 +7832,7 @@
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -7837,7 +7845,7 @@
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -7850,7 +7858,7 @@
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -7863,7 +7871,7 @@
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -7876,7 +7884,7 @@
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -7889,7 +7897,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -7902,7 +7910,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -7915,7 +7923,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -7928,7 +7936,7 @@
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -7941,7 +7949,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -7954,7 +7962,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -7967,7 +7975,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -7980,7 +7988,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -7993,7 +8001,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -8006,7 +8014,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -8019,7 +8027,7 @@
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -8032,7 +8040,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -8045,7 +8053,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -8058,7 +8066,7 @@
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -8071,7 +8079,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -8084,7 +8092,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -8097,7 +8105,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -8110,7 +8118,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -8123,7 +8131,7 @@
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -8136,7 +8144,7 @@
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -8149,7 +8157,7 @@
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -8162,7 +8170,7 @@
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -8175,7 +8183,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="2"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -8188,7 +8196,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -8201,7 +8209,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="2"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -8214,7 +8222,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -8227,7 +8235,7 @@
       <c r="J175" s="2"/>
       <c r="K175" s="2"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -8240,7 +8248,7 @@
       <c r="J176" s="2"/>
       <c r="K176" s="2"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -8253,7 +8261,7 @@
       <c r="J177" s="2"/>
       <c r="K177" s="2"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -8266,7 +8274,7 @@
       <c r="J178" s="2"/>
       <c r="K178" s="2"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -8279,7 +8287,7 @@
       <c r="J179" s="2"/>
       <c r="K179" s="2"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -8292,7 +8300,7 @@
       <c r="J180" s="2"/>
       <c r="K180" s="2"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -8305,7 +8313,7 @@
       <c r="J181" s="2"/>
       <c r="K181" s="2"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -8318,7 +8326,7 @@
       <c r="J182" s="2"/>
       <c r="K182" s="2"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -8331,7 +8339,7 @@
       <c r="J183" s="2"/>
       <c r="K183" s="2"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -8344,7 +8352,7 @@
       <c r="J184" s="2"/>
       <c r="K184" s="2"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -8357,7 +8365,7 @@
       <c r="J185" s="2"/>
       <c r="K185" s="2"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -8370,7 +8378,7 @@
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -8383,7 +8391,7 @@
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -8396,7 +8404,7 @@
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -8409,7 +8417,7 @@
       <c r="J189" s="2"/>
       <c r="K189" s="2"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -8422,7 +8430,7 @@
       <c r="J190" s="2"/>
       <c r="K190" s="2"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -8435,7 +8443,7 @@
       <c r="J191" s="2"/>
       <c r="K191" s="2"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -8448,7 +8456,7 @@
       <c r="J192" s="2"/>
       <c r="K192" s="2"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -8461,7 +8469,7 @@
       <c r="J193" s="2"/>
       <c r="K193" s="2"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -8474,7 +8482,7 @@
       <c r="J194" s="2"/>
       <c r="K194" s="2"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -8487,7 +8495,7 @@
       <c r="J195" s="2"/>
       <c r="K195" s="2"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -8500,7 +8508,7 @@
       <c r="J196" s="2"/>
       <c r="K196" s="2"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -8513,7 +8521,7 @@
       <c r="J197" s="2"/>
       <c r="K197" s="2"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -8526,7 +8534,7 @@
       <c r="J198" s="2"/>
       <c r="K198" s="2"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -8539,7 +8547,7 @@
       <c r="J199" s="2"/>
       <c r="K199" s="2"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -8552,7 +8560,7 @@
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -8565,7 +8573,7 @@
       <c r="J201" s="2"/>
       <c r="K201" s="2"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -8578,7 +8586,7 @@
       <c r="J202" s="2"/>
       <c r="K202" s="2"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -8591,7 +8599,7 @@
       <c r="J203" s="2"/>
       <c r="K203" s="2"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -8604,7 +8612,7 @@
       <c r="J204" s="2"/>
       <c r="K204" s="2"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -8617,7 +8625,7 @@
       <c r="J205" s="2"/>
       <c r="K205" s="2"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -8630,7 +8638,7 @@
       <c r="J206" s="2"/>
       <c r="K206" s="2"/>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -8643,7 +8651,7 @@
       <c r="J207" s="2"/>
       <c r="K207" s="2"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -8656,7 +8664,7 @@
       <c r="J208" s="2"/>
       <c r="K208" s="2"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -8669,7 +8677,7 @@
       <c r="J209" s="2"/>
       <c r="K209" s="2"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -8682,7 +8690,7 @@
       <c r="J210" s="2"/>
       <c r="K210" s="2"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -8695,7 +8703,7 @@
       <c r="J211" s="2"/>
       <c r="K211" s="2"/>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -8708,7 +8716,7 @@
       <c r="J212" s="2"/>
       <c r="K212" s="2"/>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -8721,7 +8729,7 @@
       <c r="J213" s="2"/>
       <c r="K213" s="2"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -8734,7 +8742,7 @@
       <c r="J214" s="2"/>
       <c r="K214" s="2"/>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -8747,7 +8755,7 @@
       <c r="J215" s="2"/>
       <c r="K215" s="2"/>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -8760,7 +8768,7 @@
       <c r="J216" s="2"/>
       <c r="K216" s="2"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -8773,7 +8781,7 @@
       <c r="J217" s="2"/>
       <c r="K217" s="2"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -8786,7 +8794,7 @@
       <c r="J218" s="2"/>
       <c r="K218" s="2"/>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -8799,7 +8807,7 @@
       <c r="J219" s="2"/>
       <c r="K219" s="2"/>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -8812,7 +8820,7 @@
       <c r="J220" s="2"/>
       <c r="K220" s="2"/>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -8825,7 +8833,7 @@
       <c r="J221" s="2"/>
       <c r="K221" s="2"/>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -8838,7 +8846,7 @@
       <c r="J222" s="2"/>
       <c r="K222" s="2"/>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
@@ -8851,7 +8859,7 @@
       <c r="J223" s="2"/>
       <c r="K223" s="2"/>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -8864,7 +8872,7 @@
       <c r="J224" s="2"/>
       <c r="K224" s="2"/>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
@@ -8877,7 +8885,7 @@
       <c r="J225" s="2"/>
       <c r="K225" s="2"/>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
@@ -8890,7 +8898,7 @@
       <c r="J226" s="2"/>
       <c r="K226" s="2"/>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>

</xml_diff>

<commit_message>
Added create and edit functionality/ changed details
</commit_message>
<xml_diff>
--- a/ExcelSheets/Tax_List_Sample.xlsx
+++ b/ExcelSheets/Tax_List_Sample.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cutte\Desktop\School\Fall2018\WebAppDevelopment\TaxWebApp\TaxWebApp\ExcelSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grace\OneDrive\Documents\GitHub\TaxWebApp\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE501960-EB13-47A8-BE80-805DB35E9879}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BEACE1-51B6-45E6-9842-2CEE56D30601}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Personals " sheetId="1" r:id="rId1"/>
+    <sheet name="Personals" sheetId="1" r:id="rId1"/>
     <sheet name="Corporate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>

</xml_diff>